<commit_message>
Updated xpath.xlsx with a link to the video
</commit_message>
<xml_diff>
--- a/xpath/xpath.xlsx
+++ b/xpath/xpath.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicol\Documents\GitHub\excel-pq\xpath\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D82FBAB6-6BD5-4DD6-8D98-629A47B331C1}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7154D5BC-5319-4363-9CF6-76380EB839A7}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9000" xr2:uid="{575935E4-1CB9-4594-AE5D-FCBEA181E11B}"/>
   </bookViews>
@@ -1348,7 +1348,7 @@
       <xdr:col>14</xdr:col>
       <xdr:colOff>556260</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>45720</xdr:rowOff>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1364,7 +1364,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2369820" y="769620"/>
-          <a:ext cx="6720840" cy="8054340"/>
+          <a:ext cx="6720840" cy="8084820"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1462,7 +1462,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>Excel Get &amp; Transform Data / From Web seems like a magic wand, but it doen't always work, as demonstrated in this video: </a:t>
+            <a:t>Excel Get &amp; Transform Data / From Web seems like a magic wand, but it doen't always work, as demonstrated in this video: https://raw.githubusercontent.com/tirlibibi17/excel-pq/master/xpath/How%20to%20get%20XPATH%20from%20element%20using%20Firefox.mp4</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -2629,15 +2629,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>388621</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>121440</xdr:rowOff>
+      <xdr:colOff>579121</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>129060</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>297181</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>7853</xdr:rowOff>
+      <xdr:colOff>487681</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>15473</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2660,7 +2660,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7703821" y="8168160"/>
+          <a:off x="7894321" y="8358660"/>
           <a:ext cx="1127760" cy="435053"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3030,7 +3030,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q39" sqref="Q39"/>
+      <selection activeCell="R18" sqref="R18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Updated xpath.xlsx with link to Reddit post
</commit_message>
<xml_diff>
--- a/xpath/xpath.xlsx
+++ b/xpath/xpath.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicol\Documents\GitHub\excel-pq\xpath\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7154D5BC-5319-4363-9CF6-76380EB839A7}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{126CA875-2E50-48F3-A770-9F2CA42EE33E}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9000" xr2:uid="{575935E4-1CB9-4594-AE5D-FCBEA181E11B}"/>
   </bookViews>
@@ -1347,8 +1347,8 @@
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>556260</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>160020</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1364,7 +1364,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2369820" y="769620"/>
-          <a:ext cx="6720840" cy="8084820"/>
+          <a:ext cx="6720840" cy="8351520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2366,7 +2366,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>/u/tirlibibi17 as a solution to </a:t>
+            <a:t>/u/tirlibibi17 as </a:t>
           </a:r>
           <a:r>
             <a:rPr lang="fr-FR" sz="1100" b="0" i="1" baseline="0">
@@ -2378,7 +2378,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>Copy and paste specific text from website url to cell</a:t>
+            <a:t>Web-scraping - solution to some cases where Power Query / From Web can't identify the different parts of a web page</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="fr-FR" sz="1100" b="0" i="0" baseline="0">
@@ -2390,7 +2390,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t> (https://old.reddit.com/r/excel/comments/9mfrcj/copy_and_paste_specific_text_from_website_url_to/)</a:t>
+            <a:t> (https://www.reddit.com/r/excel/comments/9mxxvk/webscraping_solution_to_some_cases_where_power/)</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -2630,14 +2630,14 @@
     <xdr:from>
       <xdr:col>12</xdr:col>
       <xdr:colOff>579121</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>129060</xdr:rowOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>22380</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>487681</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>15473</xdr:rowOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>91673</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2660,7 +2660,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7894321" y="8358660"/>
+          <a:off x="7894321" y="8617740"/>
           <a:ext cx="1127760" cy="435053"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3029,8 +3029,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C339B6F-C2AD-408D-BD03-785D400B411D}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="R18" sqref="R18"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="T41" sqref="T41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>